<commit_message>
Updated clustering to only use the largest 150 crises and remade clustering figures
</commit_message>
<xml_diff>
--- a/Data/AllCrises_Years12_Threshold3_LowerThreshold2_MaxDaysBelow4_minLength4_minCount50_Clustered.xlsx
+++ b/Data/AllCrises_Years12_Threshold3_LowerThreshold2_MaxDaysBelow4_minLength4_minCount50_Clustered.xlsx
@@ -1869,14 +1869,14 @@
       </c>
       <c r="AL9" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN9" t="n">
         <v>1</v>
-      </c>
-      <c r="AN9" t="n">
-        <v>0</v>
       </c>
       <c r="AO9" t="n">
         <v>0</v>
@@ -2335,10 +2335,10 @@
         </is>
       </c>
       <c r="AM12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN12" t="n">
         <v>0.002</v>
-      </c>
-      <c r="AN12" t="n">
-        <v>0</v>
       </c>
       <c r="AO12" t="n">
         <v>0.0003</v>
@@ -2641,10 +2641,10 @@
         </is>
       </c>
       <c r="AM14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN14" t="n">
         <v>0.0005</v>
-      </c>
-      <c r="AN14" t="n">
-        <v>0</v>
       </c>
       <c r="AO14" t="n">
         <v>0.0023</v>
@@ -3099,14 +3099,14 @@
       </c>
       <c r="AL17" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN17" t="n">
         <v>0.6415999999999999</v>
-      </c>
-      <c r="AN17" t="n">
-        <v>0</v>
       </c>
       <c r="AO17" t="n">
         <v>0.2599</v>
@@ -3411,10 +3411,10 @@
         </is>
       </c>
       <c r="AM19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN19" t="n">
         <v>0.0076</v>
-      </c>
-      <c r="AN19" t="n">
-        <v>0</v>
       </c>
       <c r="AO19" t="n">
         <v>0.0002</v>
@@ -3873,10 +3873,10 @@
         </is>
       </c>
       <c r="AM22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN22" t="n">
         <v>0.1767</v>
-      </c>
-      <c r="AN22" t="n">
-        <v>0</v>
       </c>
       <c r="AO22" t="n">
         <v>0</v>
@@ -4027,10 +4027,10 @@
         </is>
       </c>
       <c r="AM23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN23" t="n">
         <v>0.0248</v>
-      </c>
-      <c r="AN23" t="n">
-        <v>0</v>
       </c>
       <c r="AO23" t="n">
         <v>0.0026</v>
@@ -4487,10 +4487,10 @@
         </is>
       </c>
       <c r="AM26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN26" t="n">
         <v>0.008699999999999999</v>
-      </c>
-      <c r="AN26" t="n">
-        <v>0</v>
       </c>
       <c r="AO26" t="n">
         <v>0.0001</v>
@@ -5561,14 +5561,14 @@
       </c>
       <c r="AL33" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN33" t="n">
         <v>1</v>
-      </c>
-      <c r="AN33" t="n">
-        <v>0</v>
       </c>
       <c r="AO33" t="n">
         <v>0</v>
@@ -5719,10 +5719,10 @@
         </is>
       </c>
       <c r="AM34" t="n">
-        <v>0</v>
+        <v>0.0005</v>
       </c>
       <c r="AN34" t="n">
-        <v>0.0005</v>
+        <v>0</v>
       </c>
       <c r="AO34" t="n">
         <v>0.9994</v>
@@ -6793,14 +6793,14 @@
       </c>
       <c r="AL41" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AM41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO41" t="n">
         <v>0</v>
@@ -7871,14 +7871,14 @@
       </c>
       <c r="AL48" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AM48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO48" t="n">
         <v>0</v>
@@ -8183,10 +8183,10 @@
         </is>
       </c>
       <c r="AM50" t="n">
-        <v>0</v>
+        <v>0.2182</v>
       </c>
       <c r="AN50" t="n">
-        <v>0.2182</v>
+        <v>0</v>
       </c>
       <c r="AO50" t="n">
         <v>0.7818000000000001</v>
@@ -8337,10 +8337,10 @@
         </is>
       </c>
       <c r="AM51" t="n">
+        <v>0.0011</v>
+      </c>
+      <c r="AN51" t="n">
         <v>0.0005999999999999999</v>
-      </c>
-      <c r="AN51" t="n">
-        <v>0.0011</v>
       </c>
       <c r="AO51" t="n">
         <v>0.9971</v>
@@ -8491,10 +8491,10 @@
         </is>
       </c>
       <c r="AM52" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN52" t="n">
         <v>0.0638</v>
-      </c>
-      <c r="AN52" t="n">
-        <v>0</v>
       </c>
       <c r="AO52" t="n">
         <v>0.0027</v>
@@ -8641,14 +8641,14 @@
       </c>
       <c r="AL53" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AM53" t="n">
-        <v>0</v>
+        <v>0.9995000000000001</v>
       </c>
       <c r="AN53" t="n">
-        <v>0.9995000000000001</v>
+        <v>0</v>
       </c>
       <c r="AO53" t="n">
         <v>0.0005</v>
@@ -9565,14 +9565,14 @@
       </c>
       <c r="AL59" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM59" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN59" t="n">
         <v>0.8504</v>
-      </c>
-      <c r="AN59" t="n">
-        <v>0</v>
       </c>
       <c r="AO59" t="n">
         <v>0</v>
@@ -9873,14 +9873,14 @@
       </c>
       <c r="AL61" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AM61" t="n">
-        <v>0</v>
+        <v>0.9344</v>
       </c>
       <c r="AN61" t="n">
-        <v>0.9344</v>
+        <v>0</v>
       </c>
       <c r="AO61" t="n">
         <v>0.06560000000000001</v>
@@ -10029,10 +10029,10 @@
         </is>
       </c>
       <c r="AM62" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN62" t="n">
         <v>0.0001</v>
-      </c>
-      <c r="AN62" t="n">
-        <v>0</v>
       </c>
       <c r="AO62" t="n">
         <v>0.2734</v>
@@ -10491,10 +10491,10 @@
         </is>
       </c>
       <c r="AM65" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN65" t="n">
         <v>0.0003</v>
-      </c>
-      <c r="AN65" t="n">
-        <v>0</v>
       </c>
       <c r="AO65" t="n">
         <v>0.0021</v>
@@ -10641,14 +10641,14 @@
       </c>
       <c r="AL66" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN66" t="n">
         <v>0.9975000000000001</v>
-      </c>
-      <c r="AN66" t="n">
-        <v>0</v>
       </c>
       <c r="AO66" t="n">
         <v>0</v>
@@ -10953,10 +10953,10 @@
         </is>
       </c>
       <c r="AM68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN68" t="n">
         <v>0.1215</v>
-      </c>
-      <c r="AN68" t="n">
-        <v>0</v>
       </c>
       <c r="AO68" t="n">
         <v>0.001</v>
@@ -12027,14 +12027,14 @@
       </c>
       <c r="AL75" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN75" t="n">
         <v>0.9998</v>
-      </c>
-      <c r="AN75" t="n">
-        <v>0</v>
       </c>
       <c r="AO75" t="n">
         <v>0</v>
@@ -12181,14 +12181,14 @@
       </c>
       <c r="AL76" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AM76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN76" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO76" t="n">
         <v>0</v>
@@ -12339,10 +12339,10 @@
         </is>
       </c>
       <c r="AM77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN77" t="n">
         <v>0.0028</v>
-      </c>
-      <c r="AN77" t="n">
-        <v>0</v>
       </c>
       <c r="AO77" t="n">
         <v>0</v>
@@ -12643,14 +12643,14 @@
       </c>
       <c r="AL79" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN79" t="n">
         <v>0.9862</v>
-      </c>
-      <c r="AN79" t="n">
-        <v>0</v>
       </c>
       <c r="AO79" t="n">
         <v>0</v>
@@ -12797,14 +12797,14 @@
       </c>
       <c r="AL80" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN80" t="n">
         <v>0.964</v>
-      </c>
-      <c r="AN80" t="n">
-        <v>0</v>
       </c>
       <c r="AO80" t="n">
         <v>0</v>
@@ -12951,14 +12951,14 @@
       </c>
       <c r="AL81" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN81" t="n">
         <v>0.9627</v>
-      </c>
-      <c r="AN81" t="n">
-        <v>0</v>
       </c>
       <c r="AO81" t="n">
         <v>0</v>
@@ -13105,14 +13105,14 @@
       </c>
       <c r="AL82" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN82" t="n">
         <v>0.9999</v>
-      </c>
-      <c r="AN82" t="n">
-        <v>0</v>
       </c>
       <c r="AO82" t="n">
         <v>0</v>
@@ -13259,14 +13259,14 @@
       </c>
       <c r="AL83" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN83" t="n">
         <v>0.8427</v>
-      </c>
-      <c r="AN83" t="n">
-        <v>0</v>
       </c>
       <c r="AO83" t="n">
         <v>0</v>
@@ -13567,14 +13567,14 @@
       </c>
       <c r="AL85" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN85" t="n">
         <v>0.7561</v>
-      </c>
-      <c r="AN85" t="n">
-        <v>0</v>
       </c>
       <c r="AO85" t="n">
         <v>0.0001</v>
@@ -13721,14 +13721,14 @@
       </c>
       <c r="AL86" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN86" t="n">
         <v>0.7473</v>
-      </c>
-      <c r="AN86" t="n">
-        <v>0</v>
       </c>
       <c r="AO86" t="n">
         <v>0.0195</v>
@@ -14341,10 +14341,10 @@
         </is>
       </c>
       <c r="AM90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN90" t="n">
         <v>0.1448</v>
-      </c>
-      <c r="AN90" t="n">
-        <v>0</v>
       </c>
       <c r="AO90" t="n">
         <v>0.0002</v>
@@ -14957,10 +14957,10 @@
         </is>
       </c>
       <c r="AM94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN94" t="n">
         <v>0.0046</v>
-      </c>
-      <c r="AN94" t="n">
-        <v>0</v>
       </c>
       <c r="AO94" t="n">
         <v>0.0001</v>
@@ -15111,10 +15111,10 @@
         </is>
       </c>
       <c r="AM95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN95" t="n">
         <v>0.0009</v>
-      </c>
-      <c r="AN95" t="n">
-        <v>0</v>
       </c>
       <c r="AO95" t="n">
         <v>0.306</v>
@@ -15261,14 +15261,14 @@
       </c>
       <c r="AL96" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM96" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN96" t="n">
         <v>0.9845</v>
-      </c>
-      <c r="AN96" t="n">
-        <v>0</v>
       </c>
       <c r="AO96" t="n">
         <v>0</v>
@@ -15881,10 +15881,10 @@
         </is>
       </c>
       <c r="AM100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN100" t="n">
         <v>0.0383</v>
-      </c>
-      <c r="AN100" t="n">
-        <v>0</v>
       </c>
       <c r="AO100" t="n">
         <v>0.0203</v>
@@ -16185,14 +16185,14 @@
       </c>
       <c r="AL102" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN102" t="n">
         <v>0.9974</v>
-      </c>
-      <c r="AN102" t="n">
-        <v>0</v>
       </c>
       <c r="AO102" t="n">
         <v>0</v>
@@ -16339,14 +16339,14 @@
       </c>
       <c r="AL103" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN103" t="n">
         <v>0.9033</v>
-      </c>
-      <c r="AN103" t="n">
-        <v>0</v>
       </c>
       <c r="AO103" t="n">
         <v>0.0001</v>
@@ -16493,14 +16493,14 @@
       </c>
       <c r="AL104" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN104" t="n">
         <v>0.7695</v>
-      </c>
-      <c r="AN104" t="n">
-        <v>0</v>
       </c>
       <c r="AO104" t="n">
         <v>0</v>
@@ -16651,10 +16651,10 @@
         </is>
       </c>
       <c r="AM105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN105" t="n">
         <v>0.0001</v>
-      </c>
-      <c r="AN105" t="n">
-        <v>0</v>
       </c>
       <c r="AO105" t="n">
         <v>0.152</v>
@@ -17263,14 +17263,14 @@
       </c>
       <c r="AL109" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM109" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN109" t="n">
         <v>0.9932</v>
-      </c>
-      <c r="AN109" t="n">
-        <v>0</v>
       </c>
       <c r="AO109" t="n">
         <v>0.0004</v>
@@ -17421,10 +17421,10 @@
         </is>
       </c>
       <c r="AM110" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN110" t="n">
         <v>0.0001</v>
-      </c>
-      <c r="AN110" t="n">
-        <v>0</v>
       </c>
       <c r="AO110" t="n">
         <v>0.0011</v>
@@ -17571,14 +17571,14 @@
       </c>
       <c r="AL111" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM111" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN111" t="n">
         <v>0.9977</v>
-      </c>
-      <c r="AN111" t="n">
-        <v>0</v>
       </c>
       <c r="AO111" t="n">
         <v>0</v>
@@ -17725,14 +17725,14 @@
       </c>
       <c r="AL112" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM112" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN112" t="n">
         <v>0.9866</v>
-      </c>
-      <c r="AN112" t="n">
-        <v>0</v>
       </c>
       <c r="AO112" t="n">
         <v>0.0004</v>
@@ -18037,10 +18037,10 @@
         </is>
       </c>
       <c r="AM114" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN114" t="n">
         <v>0.001</v>
-      </c>
-      <c r="AN114" t="n">
-        <v>0</v>
       </c>
       <c r="AO114" t="n">
         <v>0.0013</v>
@@ -18345,10 +18345,10 @@
         </is>
       </c>
       <c r="AM116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN116" t="n">
         <v>0.0021</v>
-      </c>
-      <c r="AN116" t="n">
-        <v>0</v>
       </c>
       <c r="AO116" t="n">
         <v>0</v>
@@ -18499,10 +18499,10 @@
         </is>
       </c>
       <c r="AM117" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN117" t="n">
         <v>0.0001</v>
-      </c>
-      <c r="AN117" t="n">
-        <v>0</v>
       </c>
       <c r="AO117" t="n">
         <v>0</v>
@@ -18807,10 +18807,10 @@
         </is>
       </c>
       <c r="AM119" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN119" t="n">
         <v>0.2999</v>
-      </c>
-      <c r="AN119" t="n">
-        <v>0</v>
       </c>
       <c r="AO119" t="n">
         <v>0.0692</v>
@@ -18961,10 +18961,10 @@
         </is>
       </c>
       <c r="AM120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN120" t="n">
         <v>0.0005</v>
-      </c>
-      <c r="AN120" t="n">
-        <v>0</v>
       </c>
       <c r="AO120" t="n">
         <v>0.001</v>
@@ -19113,10 +19113,10 @@
         </is>
       </c>
       <c r="AM121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN121" t="n">
         <v>0.0003</v>
-      </c>
-      <c r="AN121" t="n">
-        <v>0</v>
       </c>
       <c r="AO121" t="n">
         <v>0.0035</v>
@@ -20037,10 +20037,10 @@
         </is>
       </c>
       <c r="AM127" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN127" t="n">
         <v>0.0007</v>
-      </c>
-      <c r="AN127" t="n">
-        <v>0</v>
       </c>
       <c r="AO127" t="n">
         <v>0.9527</v>
@@ -20341,14 +20341,14 @@
       </c>
       <c r="AL129" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM129" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN129" t="n">
         <v>0.9978</v>
-      </c>
-      <c r="AN129" t="n">
-        <v>0</v>
       </c>
       <c r="AO129" t="n">
         <v>0</v>
@@ -20499,10 +20499,10 @@
         </is>
       </c>
       <c r="AM130" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN130" t="n">
         <v>0.0009</v>
-      </c>
-      <c r="AN130" t="n">
-        <v>0</v>
       </c>
       <c r="AO130" t="n">
         <v>0.0185</v>
@@ -20803,14 +20803,14 @@
       </c>
       <c r="AL132" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM132" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN132" t="n">
         <v>0.862</v>
-      </c>
-      <c r="AN132" t="n">
-        <v>0</v>
       </c>
       <c r="AO132" t="n">
         <v>0</v>
@@ -21115,10 +21115,10 @@
         </is>
       </c>
       <c r="AM134" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN134" t="n">
         <v>0.0001</v>
-      </c>
-      <c r="AN134" t="n">
-        <v>0</v>
       </c>
       <c r="AO134" t="n">
         <v>0</v>
@@ -21265,14 +21265,14 @@
       </c>
       <c r="AL135" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM135" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN135" t="n">
         <v>0.9952</v>
-      </c>
-      <c r="AN135" t="n">
-        <v>0</v>
       </c>
       <c r="AO135" t="n">
         <v>0</v>
@@ -21573,14 +21573,14 @@
       </c>
       <c r="AL137" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM137" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN137" t="n">
         <v>0.9971</v>
-      </c>
-      <c r="AN137" t="n">
-        <v>0</v>
       </c>
       <c r="AO137" t="n">
         <v>0</v>
@@ -21731,10 +21731,10 @@
         </is>
       </c>
       <c r="AM138" t="n">
-        <v>0</v>
+        <v>0.0005</v>
       </c>
       <c r="AN138" t="n">
-        <v>0.0005</v>
+        <v>0</v>
       </c>
       <c r="AO138" t="n">
         <v>0.9993</v>
@@ -22039,10 +22039,10 @@
         </is>
       </c>
       <c r="AM140" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN140" t="n">
         <v>0.1353</v>
-      </c>
-      <c r="AN140" t="n">
-        <v>0</v>
       </c>
       <c r="AO140" t="n">
         <v>0</v>
@@ -22193,10 +22193,10 @@
         </is>
       </c>
       <c r="AM141" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN141" t="n">
         <v>0.0001</v>
-      </c>
-      <c r="AN141" t="n">
-        <v>0</v>
       </c>
       <c r="AO141" t="n">
         <v>0.0256</v>
@@ -22347,10 +22347,10 @@
         </is>
       </c>
       <c r="AM142" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN142" t="n">
         <v>0.0469</v>
-      </c>
-      <c r="AN142" t="n">
-        <v>0</v>
       </c>
       <c r="AO142" t="n">
         <v>0.0014</v>
@@ -22497,14 +22497,14 @@
       </c>
       <c r="AL143" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AM143" t="n">
-        <v>0</v>
+        <v>0.9792999999999999</v>
       </c>
       <c r="AN143" t="n">
-        <v>0.9792999999999999</v>
+        <v>0</v>
       </c>
       <c r="AO143" t="n">
         <v>0.0207</v>
@@ -22809,10 +22809,10 @@
         </is>
       </c>
       <c r="AM145" t="n">
+        <v>0.0003</v>
+      </c>
+      <c r="AN145" t="n">
         <v>0.0001</v>
-      </c>
-      <c r="AN145" t="n">
-        <v>0.0003</v>
       </c>
       <c r="AO145" t="n">
         <v>0.9947</v>
@@ -23575,14 +23575,14 @@
       </c>
       <c r="AL150" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AM150" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN150" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO150" t="n">
         <v>0</v>
@@ -23729,14 +23729,14 @@
       </c>
       <c r="AL151" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM151" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN151" t="n">
         <v>0.9861</v>
-      </c>
-      <c r="AN151" t="n">
-        <v>0</v>
       </c>
       <c r="AO151" t="n">
         <v>0</v>
@@ -24041,10 +24041,10 @@
         </is>
       </c>
       <c r="AM153" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN153" t="n">
         <v>0.0179</v>
-      </c>
-      <c r="AN153" t="n">
-        <v>0</v>
       </c>
       <c r="AO153" t="n">
         <v>0.0001</v>
@@ -24651,14 +24651,14 @@
       </c>
       <c r="AL157" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM157" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN157" t="n">
         <v>0.6788999999999999</v>
-      </c>
-      <c r="AN157" t="n">
-        <v>0</v>
       </c>
       <c r="AO157" t="n">
         <v>0</v>
@@ -24805,14 +24805,14 @@
       </c>
       <c r="AL158" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM158" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN158" t="n">
         <v>0.9989</v>
-      </c>
-      <c r="AN158" t="n">
-        <v>0</v>
       </c>
       <c r="AO158" t="n">
         <v>0</v>
@@ -25117,10 +25117,10 @@
         </is>
       </c>
       <c r="AM160" t="n">
-        <v>0</v>
+        <v>0.009900000000000001</v>
       </c>
       <c r="AN160" t="n">
-        <v>0.009900000000000001</v>
+        <v>0</v>
       </c>
       <c r="AO160" t="n">
         <v>0.99</v>
@@ -25271,10 +25271,10 @@
         </is>
       </c>
       <c r="AM161" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN161" t="n">
         <v>0.0002</v>
-      </c>
-      <c r="AN161" t="n">
-        <v>0</v>
       </c>
       <c r="AO161" t="n">
         <v>0</v>
@@ -25883,14 +25883,14 @@
       </c>
       <c r="AL165" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM165" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN165" t="n">
         <v>0.9997</v>
-      </c>
-      <c r="AN165" t="n">
-        <v>0</v>
       </c>
       <c r="AO165" t="n">
         <v>0</v>
@@ -26037,14 +26037,14 @@
       </c>
       <c r="AL166" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM166" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN166" t="n">
         <v>0.9475</v>
-      </c>
-      <c r="AN166" t="n">
-        <v>0</v>
       </c>
       <c r="AO166" t="n">
         <v>0</v>
@@ -26347,10 +26347,10 @@
         </is>
       </c>
       <c r="AM168" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN168" t="n">
         <v>0.0007</v>
-      </c>
-      <c r="AN168" t="n">
-        <v>0</v>
       </c>
       <c r="AO168" t="n">
         <v>0.3699</v>
@@ -26501,10 +26501,10 @@
         </is>
       </c>
       <c r="AM169" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN169" t="n">
         <v>0.4775</v>
-      </c>
-      <c r="AN169" t="n">
-        <v>0</v>
       </c>
       <c r="AO169" t="n">
         <v>0.0033</v>
@@ -26957,14 +26957,14 @@
       </c>
       <c r="AL172" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM172" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN172" t="n">
         <v>0.9842</v>
-      </c>
-      <c r="AN172" t="n">
-        <v>0</v>
       </c>
       <c r="AO172" t="n">
         <v>0</v>
@@ -27727,14 +27727,14 @@
       </c>
       <c r="AL177" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM177" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN177" t="n">
         <v>0.9778</v>
-      </c>
-      <c r="AN177" t="n">
-        <v>0</v>
       </c>
       <c r="AO177" t="n">
         <v>0</v>
@@ -27885,10 +27885,10 @@
         </is>
       </c>
       <c r="AM178" t="n">
-        <v>0</v>
+        <v>0.0003</v>
       </c>
       <c r="AN178" t="n">
-        <v>0.0003</v>
+        <v>0</v>
       </c>
       <c r="AO178" t="n">
         <v>0.992</v>
@@ -28035,14 +28035,14 @@
       </c>
       <c r="AL179" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AM179" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN179" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO179" t="n">
         <v>0</v>
@@ -28501,10 +28501,10 @@
         </is>
       </c>
       <c r="AM182" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN182" t="n">
         <v>0.0002</v>
-      </c>
-      <c r="AN182" t="n">
-        <v>0</v>
       </c>
       <c r="AO182" t="n">
         <v>0</v>
@@ -28655,10 +28655,10 @@
         </is>
       </c>
       <c r="AM183" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN183" t="n">
         <v>0.205</v>
-      </c>
-      <c r="AN183" t="n">
-        <v>0</v>
       </c>
       <c r="AO183" t="n">
         <v>0.0019</v>
@@ -28959,14 +28959,14 @@
       </c>
       <c r="AL185" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM185" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN185" t="n">
         <v>0.8443000000000001</v>
-      </c>
-      <c r="AN185" t="n">
-        <v>0</v>
       </c>
       <c r="AO185" t="n">
         <v>0.0012</v>
@@ -29117,10 +29117,10 @@
         </is>
       </c>
       <c r="AM186" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN186" t="n">
         <v>0.0057</v>
-      </c>
-      <c r="AN186" t="n">
-        <v>0</v>
       </c>
       <c r="AO186" t="n">
         <v>0.0022</v>
@@ -29271,10 +29271,10 @@
         </is>
       </c>
       <c r="AM187" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN187" t="n">
         <v>0.1457</v>
-      </c>
-      <c r="AN187" t="n">
-        <v>0</v>
       </c>
       <c r="AO187" t="n">
         <v>0.0273</v>
@@ -29575,14 +29575,14 @@
       </c>
       <c r="AL189" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM189" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN189" t="n">
         <v>0.9896</v>
-      </c>
-      <c r="AN189" t="n">
-        <v>0</v>
       </c>
       <c r="AO189" t="n">
         <v>0</v>
@@ -29729,14 +29729,14 @@
       </c>
       <c r="AL190" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM190" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN190" t="n">
         <v>0.8751</v>
-      </c>
-      <c r="AN190" t="n">
-        <v>0</v>
       </c>
       <c r="AO190" t="n">
         <v>0</v>
@@ -30653,14 +30653,14 @@
       </c>
       <c r="AL196" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AM196" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN196" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO196" t="n">
         <v>0</v>
@@ -31735,10 +31735,10 @@
         </is>
       </c>
       <c r="AM203" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN203" t="n">
         <v>0.0359</v>
-      </c>
-      <c r="AN203" t="n">
-        <v>0</v>
       </c>
       <c r="AO203" t="n">
         <v>0.003</v>
@@ -31889,10 +31889,10 @@
         </is>
       </c>
       <c r="AM204" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN204" t="n">
         <v>0.1493</v>
-      </c>
-      <c r="AN204" t="n">
-        <v>0</v>
       </c>
       <c r="AO204" t="n">
         <v>0.001</v>
@@ -32191,14 +32191,14 @@
       </c>
       <c r="AL206" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM206" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN206" t="n">
         <v>0.6816</v>
-      </c>
-      <c r="AN206" t="n">
-        <v>0</v>
       </c>
       <c r="AO206" t="n">
         <v>0.0009</v>
@@ -32349,10 +32349,10 @@
         </is>
       </c>
       <c r="AM207" t="n">
-        <v>0</v>
+        <v>0.0054</v>
       </c>
       <c r="AN207" t="n">
-        <v>0.0054</v>
+        <v>0</v>
       </c>
       <c r="AO207" t="n">
         <v>0.9944</v>
@@ -32959,14 +32959,14 @@
       </c>
       <c r="AL211" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM211" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN211" t="n">
         <v>0.9975000000000001</v>
-      </c>
-      <c r="AN211" t="n">
-        <v>0</v>
       </c>
       <c r="AO211" t="n">
         <v>0</v>
@@ -33271,10 +33271,10 @@
         </is>
       </c>
       <c r="AM213" t="n">
-        <v>0</v>
+        <v>0.0161</v>
       </c>
       <c r="AN213" t="n">
-        <v>0.0161</v>
+        <v>0</v>
       </c>
       <c r="AO213" t="n">
         <v>0.9839</v>
@@ -33421,14 +33421,14 @@
       </c>
       <c r="AL214" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM214" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN214" t="n">
         <v>0.9987</v>
-      </c>
-      <c r="AN214" t="n">
-        <v>0</v>
       </c>
       <c r="AO214" t="n">
         <v>0</v>
@@ -33579,10 +33579,10 @@
         </is>
       </c>
       <c r="AM215" t="n">
+        <v>0.0002</v>
+      </c>
+      <c r="AN215" t="n">
         <v>0.0001</v>
-      </c>
-      <c r="AN215" t="n">
-        <v>0.0002</v>
       </c>
       <c r="AO215" t="n">
         <v>0.994</v>
@@ -33729,14 +33729,14 @@
       </c>
       <c r="AL216" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AM216" t="n">
-        <v>0</v>
+        <v>0.7962</v>
       </c>
       <c r="AN216" t="n">
-        <v>0.7962</v>
+        <v>0</v>
       </c>
       <c r="AO216" t="n">
         <v>0.2038</v>
@@ -34041,10 +34041,10 @@
         </is>
       </c>
       <c r="AM218" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN218" t="n">
         <v>0.3535</v>
-      </c>
-      <c r="AN218" t="n">
-        <v>0</v>
       </c>
       <c r="AO218" t="n">
         <v>0.0056</v>
@@ -34195,10 +34195,10 @@
         </is>
       </c>
       <c r="AM219" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN219" t="n">
         <v>0.0649</v>
-      </c>
-      <c r="AN219" t="n">
-        <v>0</v>
       </c>
       <c r="AO219" t="n">
         <v>0</v>
@@ -34349,10 +34349,10 @@
         </is>
       </c>
       <c r="AM220" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN220" t="n">
         <v>0.0029</v>
-      </c>
-      <c r="AN220" t="n">
-        <v>0</v>
       </c>
       <c r="AO220" t="n">
         <v>0.0001</v>
@@ -34807,14 +34807,14 @@
       </c>
       <c r="AL223" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM223" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN223" t="n">
         <v>0.9697</v>
-      </c>
-      <c r="AN223" t="n">
-        <v>0</v>
       </c>
       <c r="AO223" t="n">
         <v>0</v>
@@ -34961,14 +34961,14 @@
       </c>
       <c r="AL224" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM224" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN224" t="n">
         <v>1</v>
-      </c>
-      <c r="AN224" t="n">
-        <v>0</v>
       </c>
       <c r="AO224" t="n">
         <v>0</v>
@@ -35119,10 +35119,10 @@
         </is>
       </c>
       <c r="AM225" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN225" t="n">
         <v>0.0005999999999999999</v>
-      </c>
-      <c r="AN225" t="n">
-        <v>0</v>
       </c>
       <c r="AO225" t="n">
         <v>0.0002</v>
@@ -35423,14 +35423,14 @@
       </c>
       <c r="AL227" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM227" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN227" t="n">
         <v>0.5317</v>
-      </c>
-      <c r="AN227" t="n">
-        <v>0</v>
       </c>
       <c r="AO227" t="n">
         <v>0</v>
@@ -35889,10 +35889,10 @@
         </is>
       </c>
       <c r="AM230" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN230" t="n">
         <v>0.0644</v>
-      </c>
-      <c r="AN230" t="n">
-        <v>0</v>
       </c>
       <c r="AO230" t="n">
         <v>0.0224</v>
@@ -36193,14 +36193,14 @@
       </c>
       <c r="AL232" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM232" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN232" t="n">
         <v>0.9848</v>
-      </c>
-      <c r="AN232" t="n">
-        <v>0</v>
       </c>
       <c r="AO232" t="n">
         <v>0</v>
@@ -36347,14 +36347,14 @@
       </c>
       <c r="AL233" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM233" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN233" t="n">
         <v>0.9987</v>
-      </c>
-      <c r="AN233" t="n">
-        <v>0</v>
       </c>
       <c r="AO233" t="n">
         <v>0</v>
@@ -36501,14 +36501,14 @@
       </c>
       <c r="AL234" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM234" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN234" t="n">
         <v>0.877</v>
-      </c>
-      <c r="AN234" t="n">
-        <v>0</v>
       </c>
       <c r="AO234" t="n">
         <v>0</v>
@@ -36813,10 +36813,10 @@
         </is>
       </c>
       <c r="AM236" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="AN236" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="AO236" t="n">
         <v>0.9995000000000001</v>
@@ -36967,10 +36967,10 @@
         </is>
       </c>
       <c r="AM237" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="AN237" t="n">
         <v>0.0849</v>
-      </c>
-      <c r="AN237" t="n">
-        <v>0.0001</v>
       </c>
       <c r="AO237" t="n">
         <v>0.9006999999999999</v>
@@ -37275,10 +37275,10 @@
         </is>
       </c>
       <c r="AM239" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN239" t="n">
         <v>0.1815</v>
-      </c>
-      <c r="AN239" t="n">
-        <v>0</v>
       </c>
       <c r="AO239" t="n">
         <v>0.08119999999999999</v>
@@ -37425,14 +37425,14 @@
       </c>
       <c r="AL240" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM240" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN240" t="n">
         <v>0.9699</v>
-      </c>
-      <c r="AN240" t="n">
-        <v>0</v>
       </c>
       <c r="AO240" t="n">
         <v>0.0001</v>
@@ -37583,10 +37583,10 @@
         </is>
       </c>
       <c r="AM241" t="n">
-        <v>0</v>
+        <v>0.0059</v>
       </c>
       <c r="AN241" t="n">
-        <v>0.0059</v>
+        <v>0</v>
       </c>
       <c r="AO241" t="n">
         <v>0.994</v>
@@ -37887,14 +37887,14 @@
       </c>
       <c r="AL243" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AM243" t="n">
-        <v>0</v>
+        <v>0.9936</v>
       </c>
       <c r="AN243" t="n">
-        <v>0.9936</v>
+        <v>0</v>
       </c>
       <c r="AO243" t="n">
         <v>0.0064</v>
@@ -38659,10 +38659,10 @@
         </is>
       </c>
       <c r="AM248" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN248" t="n">
         <v>0.008999999999999999</v>
-      </c>
-      <c r="AN248" t="n">
-        <v>0</v>
       </c>
       <c r="AO248" t="n">
         <v>0</v>
@@ -39121,10 +39121,10 @@
         </is>
       </c>
       <c r="AM251" t="n">
-        <v>0</v>
+        <v>0.0007</v>
       </c>
       <c r="AN251" t="n">
-        <v>0.0007</v>
+        <v>0</v>
       </c>
       <c r="AO251" t="n">
         <v>0.9993</v>
@@ -39271,14 +39271,14 @@
       </c>
       <c r="AL252" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM252" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN252" t="n">
         <v>0.6529</v>
-      </c>
-      <c r="AN252" t="n">
-        <v>0</v>
       </c>
       <c r="AO252" t="n">
         <v>0.0013</v>
@@ -39425,14 +39425,14 @@
       </c>
       <c r="AL253" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM253" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN253" t="n">
         <v>0.8957000000000001</v>
-      </c>
-      <c r="AN253" t="n">
-        <v>0</v>
       </c>
       <c r="AO253" t="n">
         <v>0.017</v>
@@ -39579,14 +39579,14 @@
       </c>
       <c r="AL254" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AM254" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN254" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO254" t="n">
         <v>0</v>
@@ -39733,14 +39733,14 @@
       </c>
       <c r="AL255" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM255" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN255" t="n">
         <v>0.9582000000000001</v>
-      </c>
-      <c r="AN255" t="n">
-        <v>0</v>
       </c>
       <c r="AO255" t="n">
         <v>0</v>
@@ -40045,10 +40045,10 @@
         </is>
       </c>
       <c r="AM257" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN257" t="n">
         <v>0.3198</v>
-      </c>
-      <c r="AN257" t="n">
-        <v>0</v>
       </c>
       <c r="AO257" t="n">
         <v>0.0009</v>
@@ -40199,10 +40199,10 @@
         </is>
       </c>
       <c r="AM258" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="AN258" t="n">
-        <v>0.0002</v>
+        <v>0</v>
       </c>
       <c r="AO258" t="n">
         <v>0.9985000000000001</v>
@@ -40661,10 +40661,10 @@
         </is>
       </c>
       <c r="AM261" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN261" t="n">
         <v>0.1093</v>
-      </c>
-      <c r="AN261" t="n">
-        <v>0</v>
       </c>
       <c r="AO261" t="n">
         <v>0.0003</v>
@@ -40969,10 +40969,10 @@
         </is>
       </c>
       <c r="AM263" t="n">
-        <v>0</v>
+        <v>0.0226</v>
       </c>
       <c r="AN263" t="n">
-        <v>0.0226</v>
+        <v>0</v>
       </c>
       <c r="AO263" t="n">
         <v>0.9774</v>
@@ -41123,10 +41123,10 @@
         </is>
       </c>
       <c r="AM264" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN264" t="n">
         <v>0.0116</v>
-      </c>
-      <c r="AN264" t="n">
-        <v>0</v>
       </c>
       <c r="AO264" t="n">
         <v>0.0001</v>
@@ -41893,10 +41893,10 @@
         </is>
       </c>
       <c r="AM269" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN269" t="n">
         <v>0.0018</v>
-      </c>
-      <c r="AN269" t="n">
-        <v>0</v>
       </c>
       <c r="AO269" t="n">
         <v>0.0064</v>
@@ -42047,10 +42047,10 @@
         </is>
       </c>
       <c r="AM270" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN270" t="n">
         <v>0.0747</v>
-      </c>
-      <c r="AN270" t="n">
-        <v>0</v>
       </c>
       <c r="AO270" t="n">
         <v>0</v>
@@ -42199,10 +42199,10 @@
         </is>
       </c>
       <c r="AM271" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN271" t="n">
         <v>0.0005</v>
-      </c>
-      <c r="AN271" t="n">
-        <v>0</v>
       </c>
       <c r="AO271" t="n">
         <v>0.8225</v>
@@ -42353,10 +42353,10 @@
         </is>
       </c>
       <c r="AM272" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN272" t="n">
         <v>0.0291</v>
-      </c>
-      <c r="AN272" t="n">
-        <v>0</v>
       </c>
       <c r="AO272" t="n">
         <v>0.08550000000000001</v>
@@ -42657,14 +42657,14 @@
       </c>
       <c r="AL274" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM274" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN274" t="n">
         <v>0.5158</v>
-      </c>
-      <c r="AN274" t="n">
-        <v>0</v>
       </c>
       <c r="AO274" t="n">
         <v>0</v>
@@ -43273,14 +43273,14 @@
       </c>
       <c r="AL278" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AM278" t="n">
-        <v>0</v>
+        <v>0.9207</v>
       </c>
       <c r="AN278" t="n">
-        <v>0.9207</v>
+        <v>0</v>
       </c>
       <c r="AO278" t="n">
         <v>0.0793</v>
@@ -43585,10 +43585,10 @@
         </is>
       </c>
       <c r="AM280" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN280" t="n">
         <v>0.1132</v>
-      </c>
-      <c r="AN280" t="n">
-        <v>0</v>
       </c>
       <c r="AO280" t="n">
         <v>0.0001</v>
@@ -44199,10 +44199,10 @@
         </is>
       </c>
       <c r="AM284" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN284" t="n">
         <v>0.0051</v>
-      </c>
-      <c r="AN284" t="n">
-        <v>0</v>
       </c>
       <c r="AO284" t="n">
         <v>0.0002</v>
@@ -44353,10 +44353,10 @@
         </is>
       </c>
       <c r="AM285" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN285" t="n">
         <v>0.3416</v>
-      </c>
-      <c r="AN285" t="n">
-        <v>0</v>
       </c>
       <c r="AO285" t="n">
         <v>0.0005</v>
@@ -44507,10 +44507,10 @@
         </is>
       </c>
       <c r="AM286" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN286" t="n">
         <v>0.0025</v>
-      </c>
-      <c r="AN286" t="n">
-        <v>0</v>
       </c>
       <c r="AO286" t="n">
         <v>0.5296</v>
@@ -44661,10 +44661,10 @@
         </is>
       </c>
       <c r="AM287" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN287" t="n">
         <v>0.0002</v>
-      </c>
-      <c r="AN287" t="n">
-        <v>0</v>
       </c>
       <c r="AO287" t="n">
         <v>0.0002</v>
@@ -44811,14 +44811,14 @@
       </c>
       <c r="AL288" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM288" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN288" t="n">
         <v>0.982</v>
-      </c>
-      <c r="AN288" t="n">
-        <v>0</v>
       </c>
       <c r="AO288" t="n">
         <v>0</v>
@@ -45277,10 +45277,10 @@
         </is>
       </c>
       <c r="AM291" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN291" t="n">
         <v>0.009599999999999999</v>
-      </c>
-      <c r="AN291" t="n">
-        <v>0</v>
       </c>
       <c r="AO291" t="n">
         <v>0.0005</v>
@@ -45585,10 +45585,10 @@
         </is>
       </c>
       <c r="AM293" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN293" t="n">
         <v>0.002</v>
-      </c>
-      <c r="AN293" t="n">
-        <v>0</v>
       </c>
       <c r="AO293" t="n">
         <v>0.1819</v>
@@ -45893,10 +45893,10 @@
         </is>
       </c>
       <c r="AM295" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN295" t="n">
         <v>0.0028</v>
-      </c>
-      <c r="AN295" t="n">
-        <v>0</v>
       </c>
       <c r="AO295" t="n">
         <v>0.0607</v>
@@ -46043,14 +46043,14 @@
       </c>
       <c r="AL296" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM296" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN296" t="n">
         <v>0.9363</v>
-      </c>
-      <c r="AN296" t="n">
-        <v>0</v>
       </c>
       <c r="AO296" t="n">
         <v>0</v>
@@ -46197,14 +46197,14 @@
       </c>
       <c r="AL297" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM297" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN297" t="n">
         <v>0.9451000000000001</v>
-      </c>
-      <c r="AN297" t="n">
-        <v>0</v>
       </c>
       <c r="AO297" t="n">
         <v>0</v>
@@ -46505,14 +46505,14 @@
       </c>
       <c r="AL299" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM299" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN299" t="n">
         <v>0.8791</v>
-      </c>
-      <c r="AN299" t="n">
-        <v>0</v>
       </c>
       <c r="AO299" t="n">
         <v>0.0005999999999999999</v>
@@ -47121,14 +47121,14 @@
       </c>
       <c r="AL303" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="AM303" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN303" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO303" t="n">
         <v>0</v>
@@ -47433,10 +47433,10 @@
         </is>
       </c>
       <c r="AM305" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN305" t="n">
         <v>0.0002</v>
-      </c>
-      <c r="AN305" t="n">
-        <v>0</v>
       </c>
       <c r="AO305" t="n">
         <v>0.894</v>
@@ -47737,14 +47737,14 @@
       </c>
       <c r="AL307" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM307" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN307" t="n">
         <v>0.4823</v>
-      </c>
-      <c r="AN307" t="n">
-        <v>0</v>
       </c>
       <c r="AO307" t="n">
         <v>0.046</v>
@@ -48045,14 +48045,14 @@
       </c>
       <c r="AL309" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM309" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN309" t="n">
         <v>0.8466</v>
-      </c>
-      <c r="AN309" t="n">
-        <v>0</v>
       </c>
       <c r="AO309" t="n">
         <v>0</v>
@@ -48511,10 +48511,10 @@
         </is>
       </c>
       <c r="AM312" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN312" t="n">
         <v>0.008800000000000001</v>
-      </c>
-      <c r="AN312" t="n">
-        <v>0</v>
       </c>
       <c r="AO312" t="n">
         <v>0.8044</v>
@@ -48815,14 +48815,14 @@
       </c>
       <c r="AL314" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM314" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN314" t="n">
         <v>0.9994</v>
-      </c>
-      <c r="AN314" t="n">
-        <v>0</v>
       </c>
       <c r="AO314" t="n">
         <v>0</v>
@@ -48973,10 +48973,10 @@
         </is>
       </c>
       <c r="AM315" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN315" t="n">
         <v>0.0002</v>
-      </c>
-      <c r="AN315" t="n">
-        <v>0</v>
       </c>
       <c r="AO315" t="n">
         <v>0.8679</v>
@@ -49123,14 +49123,14 @@
       </c>
       <c r="AL316" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM316" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN316" t="n">
         <v>0.9999</v>
-      </c>
-      <c r="AN316" t="n">
-        <v>0</v>
       </c>
       <c r="AO316" t="n">
         <v>0</v>
@@ -49589,10 +49589,10 @@
         </is>
       </c>
       <c r="AM319" t="n">
-        <v>0</v>
+        <v>0.3395</v>
       </c>
       <c r="AN319" t="n">
-        <v>0.3395</v>
+        <v>0</v>
       </c>
       <c r="AO319" t="n">
         <v>0.6605</v>
@@ -49739,14 +49739,14 @@
       </c>
       <c r="AL320" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="AM320" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN320" t="n">
         <v>0.968</v>
-      </c>
-      <c r="AN320" t="n">
-        <v>0</v>
       </c>
       <c r="AO320" t="n">
         <v>0</v>
@@ -49897,10 +49897,10 @@
         </is>
       </c>
       <c r="AM321" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN321" t="n">
         <v>0.0808</v>
-      </c>
-      <c r="AN321" t="n">
-        <v>0</v>
       </c>
       <c r="AO321" t="n">
         <v>0.0008</v>

</xml_diff>